<commit_message>
test: expand tests to cover remaining repeat block expansion logic
</commit_message>
<xml_diff>
--- a/tests/testthat/files/expand_surveycto_config/example_cto_form_repeat_appended.xlsx
+++ b/tests/testthat/files/expand_surveycto_config/example_cto_form_repeat_appended.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="368">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t xml:space="preserve">end repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name5</t>
   </si>
   <si>
     <t xml:space="preserve">integer</t>
@@ -3785,10 +3791,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.78"/>
@@ -4102,14 +4108,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>32</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -4153,10 +4155,14 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -4200,14 +4206,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="9"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -4251,10 +4253,14 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -4297,7 +4303,9 @@
       <c r="AQ9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -4342,9 +4350,15 @@
       <c r="AQ10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -4387,7 +4401,9 @@
       <c r="AQ11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
@@ -12846,9 +12862,141 @@
       <c r="AP199" s="11"/>
       <c r="AQ199" s="11"/>
     </row>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A200" s="7"/>
+      <c r="B200" s="7"/>
+      <c r="C200" s="8"/>
+      <c r="D200" s="9"/>
+      <c r="E200" s="7"/>
+      <c r="F200" s="7"/>
+      <c r="G200" s="10"/>
+      <c r="H200" s="10"/>
+      <c r="I200" s="10"/>
+      <c r="J200" s="10"/>
+      <c r="K200" s="7"/>
+      <c r="L200" s="7"/>
+      <c r="M200" s="7"/>
+      <c r="N200" s="7"/>
+      <c r="O200" s="7"/>
+      <c r="P200" s="7"/>
+      <c r="Q200" s="7"/>
+      <c r="R200" s="7"/>
+      <c r="S200" s="7"/>
+      <c r="T200" s="7"/>
+      <c r="U200" s="7"/>
+      <c r="V200" s="7"/>
+      <c r="W200" s="7"/>
+      <c r="X200" s="11"/>
+      <c r="Y200" s="11"/>
+      <c r="Z200" s="11"/>
+      <c r="AA200" s="11"/>
+      <c r="AB200" s="11"/>
+      <c r="AC200" s="11"/>
+      <c r="AD200" s="11"/>
+      <c r="AE200" s="11"/>
+      <c r="AF200" s="11"/>
+      <c r="AG200" s="11"/>
+      <c r="AH200" s="11"/>
+      <c r="AI200" s="11"/>
+      <c r="AJ200" s="11"/>
+      <c r="AK200" s="11"/>
+      <c r="AL200" s="11"/>
+      <c r="AM200" s="11"/>
+      <c r="AN200" s="11"/>
+      <c r="AO200" s="11"/>
+      <c r="AP200" s="11"/>
+      <c r="AQ200" s="11"/>
+    </row>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A201" s="7"/>
+      <c r="B201" s="7"/>
+      <c r="C201" s="8"/>
+      <c r="D201" s="9"/>
+      <c r="E201" s="7"/>
+      <c r="F201" s="7"/>
+      <c r="G201" s="10"/>
+      <c r="H201" s="10"/>
+      <c r="I201" s="10"/>
+      <c r="J201" s="10"/>
+      <c r="K201" s="7"/>
+      <c r="L201" s="7"/>
+      <c r="M201" s="7"/>
+      <c r="N201" s="7"/>
+      <c r="O201" s="7"/>
+      <c r="P201" s="7"/>
+      <c r="Q201" s="7"/>
+      <c r="R201" s="7"/>
+      <c r="S201" s="7"/>
+      <c r="T201" s="7"/>
+      <c r="U201" s="7"/>
+      <c r="V201" s="7"/>
+      <c r="W201" s="7"/>
+      <c r="X201" s="11"/>
+      <c r="Y201" s="11"/>
+      <c r="Z201" s="11"/>
+      <c r="AA201" s="11"/>
+      <c r="AB201" s="11"/>
+      <c r="AC201" s="11"/>
+      <c r="AD201" s="11"/>
+      <c r="AE201" s="11"/>
+      <c r="AF201" s="11"/>
+      <c r="AG201" s="11"/>
+      <c r="AH201" s="11"/>
+      <c r="AI201" s="11"/>
+      <c r="AJ201" s="11"/>
+      <c r="AK201" s="11"/>
+      <c r="AL201" s="11"/>
+      <c r="AM201" s="11"/>
+      <c r="AN201" s="11"/>
+      <c r="AO201" s="11"/>
+      <c r="AP201" s="11"/>
+      <c r="AQ201" s="11"/>
+    </row>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A202" s="7"/>
+      <c r="B202" s="7"/>
+      <c r="C202" s="8"/>
+      <c r="D202" s="9"/>
+      <c r="E202" s="7"/>
+      <c r="F202" s="7"/>
+      <c r="G202" s="10"/>
+      <c r="H202" s="10"/>
+      <c r="I202" s="10"/>
+      <c r="J202" s="10"/>
+      <c r="K202" s="7"/>
+      <c r="L202" s="7"/>
+      <c r="M202" s="7"/>
+      <c r="N202" s="7"/>
+      <c r="O202" s="7"/>
+      <c r="P202" s="7"/>
+      <c r="Q202" s="7"/>
+      <c r="R202" s="7"/>
+      <c r="S202" s="7"/>
+      <c r="T202" s="7"/>
+      <c r="U202" s="7"/>
+      <c r="V202" s="7"/>
+      <c r="W202" s="7"/>
+      <c r="X202" s="11"/>
+      <c r="Y202" s="11"/>
+      <c r="Z202" s="11"/>
+      <c r="AA202" s="11"/>
+      <c r="AB202" s="11"/>
+      <c r="AC202" s="11"/>
+      <c r="AD202" s="11"/>
+      <c r="AE202" s="11"/>
+      <c r="AF202" s="11"/>
+      <c r="AG202" s="11"/>
+      <c r="AH202" s="11"/>
+      <c r="AI202" s="11"/>
+      <c r="AJ202" s="11"/>
+      <c r="AK202" s="11"/>
+      <c r="AL202" s="11"/>
+      <c r="AM202" s="11"/>
+      <c r="AN202" s="11"/>
+      <c r="AO202" s="11"/>
+      <c r="AP202" s="11"/>
+      <c r="AQ202" s="11"/>
+    </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -13269,9 +13417,9 @@
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -13651,177 +13799,177 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="B1:C622 F1:F622 I1:I622">
+  <conditionalFormatting sqref="B1:C625 F1:F625 I1:I625">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622 I1:I622 O1:O622">
+  <conditionalFormatting sqref="B1:C625 I1:I625 O1:O625">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D622 F1:F622">
+  <conditionalFormatting sqref="B1:D625 F1:F625">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D622 G1:H622">
+  <conditionalFormatting sqref="B1:D625 G1:H625">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D622 G1:H622">
+  <conditionalFormatting sqref="B1:D625 G1:H625">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622 F1:F622">
+  <conditionalFormatting sqref="B1:C625 F1:F625">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B622 F1:F622">
+  <conditionalFormatting sqref="B1:B625 F1:F625">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622">
+  <conditionalFormatting sqref="B1:C625">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>$A1="note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622">
+  <conditionalFormatting sqref="B1:C625">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>$A1="barcode"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622">
+  <conditionalFormatting sqref="B1:C625">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B622 N1:N622">
+  <conditionalFormatting sqref="B1:B625 N1:N625">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622 F1:F622">
+  <conditionalFormatting sqref="B1:C625 F1:F625">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622 F1:F622">
+  <conditionalFormatting sqref="B1:C625 F1:F625">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C622">
+  <conditionalFormatting sqref="B1:C625">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>$A1="note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>$A1="barcode"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
       <formula>$A1="end repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>$A1="end group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W622">
+  <conditionalFormatting sqref="A1:W625">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B622">
+  <conditionalFormatting sqref="B1:B625">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B622 F1:F622">
+  <conditionalFormatting sqref="B1:B625 F1:F625">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -13849,7 +13997,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.44"/>
@@ -13859,19 +14007,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -13896,13 +14044,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -13929,13 +14077,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -21850,7 +21998,7 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.33"/>
@@ -21862,25 +22010,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H1" s="17"/>
       <c r="I1" s="5"/>
@@ -21904,10 +22052,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C2" s="19" t="n">
         <v>11111</v>
@@ -21915,10 +22063,10 @@
       <c r="D2" s="14"/>
       <c r="E2" s="20"/>
       <c r="F2" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -22941,14 +23089,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="1" style="0" width="36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="22"/>
@@ -23014,7 +23162,7 @@
     </row>
     <row r="3" customFormat="false" ht="96.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="22"/>
@@ -23089,13 +23237,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>4</v>
@@ -23110,7 +23258,7 @@
         <v>7</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>8</v>
@@ -23125,7 +23273,7 @@
         <v>11</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>12</v>
@@ -23146,13 +23294,13 @@
         <v>17</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>22</v>
@@ -23172,94 +23320,94 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="O6" s="26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R6" s="25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="S6" s="25" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="T6" s="25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="W6" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="X6" s="25" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Y6" s="25" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="Z6" s="25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AA6" s="26" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AB6" s="25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AC6" s="25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AD6" s="25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23296,7 +23444,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
@@ -23365,10 +23513,10 @@
         <v>23</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -23403,17 +23551,17 @@
         <v>23</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
       <c r="H11" s="30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="30"/>
@@ -23440,13 +23588,13 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -23478,13 +23626,13 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -23516,13 +23664,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -23554,20 +23702,20 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
       <c r="H15" s="30" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
@@ -23594,20 +23742,20 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
@@ -23634,20 +23782,20 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
@@ -23674,20 +23822,20 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="30" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
@@ -23714,20 +23862,20 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
       <c r="H19" s="30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I19" s="30"/>
       <c r="J19" s="30"/>
@@ -23754,20 +23902,20 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
       <c r="H20" s="30" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
@@ -23794,20 +23942,20 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I21" s="30"/>
       <c r="J21" s="30"/>
@@ -23834,20 +23982,20 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I22" s="30"/>
       <c r="J22" s="30"/>
@@ -23874,20 +24022,20 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
       <c r="H23" s="30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="30"/>
@@ -23914,20 +24062,20 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
       <c r="H24" s="30" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
@@ -23954,20 +24102,20 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
@@ -23994,20 +24142,20 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
       <c r="G26" s="30"/>
       <c r="H26" s="30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I26" s="30"/>
       <c r="J26" s="30"/>
@@ -24034,20 +24182,20 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
       <c r="H27" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I27" s="30"/>
       <c r="J27" s="30"/>
@@ -24074,20 +24222,20 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
       <c r="H28" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
@@ -24114,13 +24262,13 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
@@ -24152,20 +24300,20 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
       <c r="H30" s="30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I30" s="30"/>
       <c r="J30" s="30"/>
@@ -24192,20 +24340,20 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
       <c r="H31" s="30" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I31" s="30"/>
       <c r="J31" s="30"/>
@@ -24232,20 +24380,20 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
       <c r="H32" s="30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
@@ -24272,20 +24420,20 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
       <c r="H33" s="30" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I33" s="30"/>
       <c r="J33" s="30"/>
@@ -24312,20 +24460,20 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
       <c r="G34" s="30"/>
       <c r="H34" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I34" s="30"/>
       <c r="J34" s="30"/>
@@ -24352,20 +24500,20 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
       <c r="G35" s="30"/>
       <c r="H35" s="30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
@@ -24392,20 +24540,20 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
       <c r="G36" s="30"/>
       <c r="H36" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I36" s="30"/>
       <c r="J36" s="30"/>
@@ -24432,20 +24580,20 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
@@ -24472,13 +24620,13 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="30" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30"/>
@@ -24510,13 +24658,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D39" s="30"/>
       <c r="E39" s="30"/>
@@ -24548,13 +24696,13 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="30" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30"/>
@@ -24586,13 +24734,13 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="30"/>
@@ -24624,13 +24772,13 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30"/>
@@ -24662,20 +24810,20 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="30" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
       <c r="G43" s="30"/>
       <c r="H43" s="30" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I43" s="30"/>
       <c r="J43" s="30"/>
@@ -24702,13 +24850,13 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="30" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30"/>
@@ -24740,20 +24888,20 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="30" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="30"/>
       <c r="F45" s="30"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I45" s="30"/>
       <c r="J45" s="30"/>
@@ -24780,13 +24928,13 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30"/>
@@ -24818,20 +24966,20 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
       <c r="H47" s="30" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I47" s="30"/>
       <c r="J47" s="30"/>
@@ -24858,20 +25006,20 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30"/>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
       <c r="H48" s="30" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I48" s="30"/>
       <c r="J48" s="30"/>
@@ -24898,20 +25046,20 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30"/>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
       <c r="H49" s="30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I49" s="30"/>
       <c r="J49" s="30"/>
@@ -24938,13 +25086,13 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="30" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -24976,13 +25124,13 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="30" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30"/>
@@ -25014,13 +25162,13 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="30" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -25055,10 +25203,10 @@
         <v>18</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D53" s="30"/>
       <c r="E53" s="30"/>
@@ -25090,10 +25238,10 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="30" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="30"/>
@@ -25126,10 +25274,10 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="30" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="30"/>
@@ -25162,10 +25310,10 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="30" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="30"/>
@@ -25198,10 +25346,10 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="30" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="30"/>
@@ -25234,10 +25382,10 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="30"/>
@@ -25270,10 +25418,10 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="30" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C59" s="31"/>
       <c r="D59" s="30"/>
@@ -25306,10 +25454,10 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="30" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="30"/>
@@ -25342,10 +25490,10 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="30" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="30"/>
@@ -25378,10 +25526,10 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="30" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="30"/>
@@ -25399,7 +25547,7 @@
       <c r="P62" s="30"/>
       <c r="Q62" s="30"/>
       <c r="R62" s="30" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="S62" s="30"/>
       <c r="T62" s="30"/>
@@ -25416,10 +25564,10 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="30" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="30"/>
@@ -25437,7 +25585,7 @@
       <c r="P63" s="30"/>
       <c r="Q63" s="30"/>
       <c r="R63" s="30" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="S63" s="30"/>
       <c r="T63" s="30"/>
@@ -25454,10 +25602,10 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="30"/>
@@ -25465,7 +25613,7 @@
       <c r="F64" s="30"/>
       <c r="G64" s="30"/>
       <c r="H64" s="30" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I64" s="30"/>
       <c r="J64" s="30"/>
@@ -25492,10 +25640,10 @@
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="30"/>
@@ -25503,7 +25651,7 @@
       <c r="F65" s="30"/>
       <c r="G65" s="30"/>
       <c r="H65" s="30" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I65" s="30"/>
       <c r="J65" s="30"/>
@@ -25530,10 +25678,10 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="30"/>
@@ -25541,7 +25689,7 @@
       <c r="F66" s="30"/>
       <c r="G66" s="30"/>
       <c r="H66" s="30" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="I66" s="30"/>
       <c r="J66" s="30"/>
@@ -25568,10 +25716,10 @@
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="30"/>
@@ -25579,7 +25727,7 @@
       <c r="F67" s="30"/>
       <c r="G67" s="30"/>
       <c r="H67" s="30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I67" s="30"/>
       <c r="J67" s="30"/>
@@ -25606,13 +25754,13 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -25644,7 +25792,7 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B69" s="30"/>
       <c r="C69" s="31"/>
@@ -25678,10 +25826,10 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="30" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="30"/>
@@ -25717,10 +25865,10 @@
         <v>26</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -25752,7 +25900,7 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B72" s="30"/>
       <c r="C72" s="31"/>
@@ -25789,7 +25937,7 @@
         <v>29</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="30"/>
@@ -25825,10 +25973,10 @@
         <v>26</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30"/>
@@ -25862,7 +26010,7 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B75" s="30"/>
       <c r="C75" s="31"/>
@@ -25899,7 +26047,7 @@
         <v>29</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="30"/>
@@ -25932,10 +26080,10 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="30" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C77" s="31"/>
       <c r="D77" s="30"/>
@@ -25968,10 +26116,10 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="30" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="30"/>
@@ -26004,10 +26152,10 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="30" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C79" s="31"/>
       <c r="D79" s="30"/>
@@ -26015,7 +26163,7 @@
       <c r="F79" s="30"/>
       <c r="G79" s="30"/>
       <c r="H79" s="30" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I79" s="30"/>
       <c r="J79" s="30"/>
@@ -26042,10 +26190,10 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="30" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C80" s="31"/>
       <c r="D80" s="30"/>
@@ -26053,7 +26201,7 @@
       <c r="F80" s="30"/>
       <c r="G80" s="30"/>
       <c r="H80" s="30" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I80" s="30"/>
       <c r="J80" s="30"/>
@@ -26080,10 +26228,10 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="30" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C81" s="31"/>
       <c r="D81" s="30"/>
@@ -26091,7 +26239,7 @@
       <c r="F81" s="30"/>
       <c r="G81" s="30"/>
       <c r="H81" s="30" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="I81" s="30"/>
       <c r="J81" s="30"/>
@@ -26121,7 +26269,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B83" s="34"/>
       <c r="C83" s="35"/>
@@ -26158,27 +26306,27 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="37" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B85" s="37" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C85" s="37" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D85" s="37" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="38" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D86" s="38" t="n">
         <v>2</v>
@@ -26186,10 +26334,10 @@
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="38" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C87" s="39" t="str">
         <f aca="false">"3 - 2"</f>
@@ -26201,13 +26349,13 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="38" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D88" s="38" t="n">
         <v>6</v>
@@ -26215,13 +26363,13 @@
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="38" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D89" s="38" t="n">
         <v>5</v>
@@ -26229,13 +26377,13 @@
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="38" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B90" s="38" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D90" s="38" t="n">
         <v>1</v>
@@ -26243,128 +26391,128 @@
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="38" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D91" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="38" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B92" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C92" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="D92" s="38" t="s">
         <v>228</v>
-      </c>
-      <c r="C92" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="D92" s="38" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="38" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C93" s="38" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D93" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="38" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="38" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B95" s="38" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C95" s="38" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="38" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C96" s="38" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D96" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="38" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B97" s="38" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D97" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="38" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B98" s="38" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C98" s="38" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D98" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="38" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B99" s="38" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C99" s="38" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D99" s="38" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26376,540 +26524,540 @@
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="36"/>
       <c r="B101" s="37" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C101" s="37" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D101" s="36"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="36"/>
       <c r="B102" s="40" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C102" s="41" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D102" s="36"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="36"/>
       <c r="B103" s="41" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C103" s="41" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D103" s="36"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="36"/>
       <c r="B104" s="41" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C104" s="41" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D104" s="36"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="36"/>
       <c r="B105" s="41" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C105" s="41" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D105" s="36"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="36"/>
       <c r="B106" s="41" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C106" s="41" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D106" s="36"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="36"/>
       <c r="B107" s="41" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C107" s="41" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D107" s="36"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="36"/>
       <c r="B108" s="41" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C108" s="41" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D108" s="36"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="36"/>
       <c r="B109" s="41" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C109" s="41" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D109" s="36"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="36"/>
       <c r="B110" s="41" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C110" s="41" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D110" s="36"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="36"/>
       <c r="B111" s="41" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C111" s="41" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D111" s="36"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="36"/>
       <c r="B112" s="41" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C112" s="41" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D112" s="36"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="36"/>
       <c r="B113" s="41" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C113" s="41" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D113" s="36"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="36"/>
       <c r="B114" s="41" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C114" s="41" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D114" s="36"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="36"/>
       <c r="B115" s="41" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C115" s="41" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D115" s="36"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="36"/>
       <c r="B116" s="41" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D116" s="36"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="36"/>
       <c r="B117" s="41" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C117" s="41" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D117" s="36"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="36"/>
       <c r="B118" s="41" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C118" s="41" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D118" s="36"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="36"/>
       <c r="B119" s="41" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C119" s="41" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D119" s="36"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="36"/>
       <c r="B120" s="41" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C120" s="41" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D120" s="36"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="36"/>
       <c r="B121" s="41" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C121" s="41" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D121" s="36"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="36"/>
       <c r="B122" s="41" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C122" s="41" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D122" s="36"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="36"/>
       <c r="B123" s="41" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C123" s="41" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D123" s="36"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="36"/>
       <c r="B124" s="41" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C124" s="41" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D124" s="36"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="36"/>
       <c r="B125" s="41" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C125" s="41" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D125" s="36"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="36"/>
       <c r="B126" s="41" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C126" s="41" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D126" s="36"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="36"/>
       <c r="B127" s="41" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C127" s="41" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D127" s="36"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="36"/>
       <c r="B128" s="41" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C128" s="41" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D128" s="36"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="36"/>
       <c r="B129" s="42" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C129" s="42" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D129" s="36"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="36"/>
       <c r="B130" s="42" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C130" s="42" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D130" s="36"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="36"/>
       <c r="B131" s="42" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C131" s="42" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D131" s="36"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="36"/>
       <c r="B132" s="42" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C132" s="42" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D132" s="36"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="36"/>
       <c r="B133" s="42" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C133" s="42" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D133" s="36"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="36"/>
       <c r="B134" s="42" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C134" s="42" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D134" s="36"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="36"/>
       <c r="B135" s="42" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C135" s="42" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D135" s="36"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="36"/>
       <c r="B136" s="42" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C136" s="42" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D136" s="36"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="36"/>
       <c r="B137" s="42" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C137" s="42" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D137" s="36"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="36"/>
       <c r="B138" s="42" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C138" s="42" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D138" s="36"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="36"/>
       <c r="B139" s="42" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C139" s="42" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D139" s="36"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="36"/>
       <c r="B140" s="42" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C140" s="42" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D140" s="36"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="36"/>
       <c r="B141" s="42" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C141" s="42" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D141" s="36"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="36"/>
       <c r="B142" s="42" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C142" s="42" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D142" s="36"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="36"/>
       <c r="B143" s="42" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C143" s="42" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D143" s="36"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="36"/>
       <c r="B144" s="42" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C144" s="42" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D144" s="36"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="36"/>
       <c r="B145" s="42" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C145" s="42" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D145" s="36"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="36"/>
       <c r="B146" s="42" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C146" s="42" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D146" s="36"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="36"/>
       <c r="B147" s="42" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C147" s="42" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D147" s="36"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="36"/>
       <c r="B148" s="42" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C148" s="42" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D148" s="36"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="36"/>
       <c r="B149" s="42" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C149" s="42" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D149" s="36"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="36"/>
       <c r="B150" s="42" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C150" s="42" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D150" s="36"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="36"/>
       <c r="B151" s="42" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C151" s="42" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D151" s="36"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="36"/>
       <c r="B152" s="42" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C152" s="42" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D152" s="36"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="36"/>
       <c r="B153" s="42" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C153" s="42" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D153" s="36"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="36"/>
       <c r="B154" s="42" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C154" s="42" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D154" s="36"/>
     </row>
@@ -28678,7 +28826,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="10.56"/>
@@ -28686,7 +28834,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="11"/>
@@ -28744,7 +28892,7 @@
     </row>
     <row r="3" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="11"/>
@@ -28802,25 +28950,25 @@
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -28844,25 +28992,25 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="43"/>
@@ -29905,7 +30053,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
@@ -29913,7 +30061,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="44" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="45"/>
@@ -29971,7 +30119,7 @@
     </row>
     <row r="3" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="46" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="45"/>
@@ -30029,22 +30177,22 @@
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="47" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3"/>
@@ -30069,22 +30217,22 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>

</xml_diff>